<commit_message>
Get data from formularios instead of aggregated excel file. Run data loading and QC with new bwayo_species_2 and alt_to_name dictionary.
</commit_message>
<xml_diff>
--- a/data/formularios/FormularioDAPAugier.xlsx
+++ b/data/formularios/FormularioDAPAugier.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\drive1\Haiti_DR_Woodfuel_Mapping2016\FieldWork_SepOct2019\Plots\Augier\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2EB537-8D56-4D94-98C4-EF155F38DB4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-16335" yWindow="1140" windowWidth="15330" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +14,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$P$14</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="66">
   <si>
     <t>Lat_v1</t>
   </si>
@@ -221,11 +220,14 @@
   <si>
     <t>Calebasse</t>
   </si>
+  <si>
+    <t>Augier</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -340,42 +342,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -383,23 +385,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -414,7 +416,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -464,19 +466,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,12 +481,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Salida" xfId="1" builtinId="21"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -555,7 +557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,7 +609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,76 +834,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4"/>
-    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="11.5" style="4"/>
+    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="4"/>
     <col min="6" max="6" width="15" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="13" style="4" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" style="4" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="4" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" style="4" customWidth="1"/>
     <col min="17" max="17" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="5"/>
-    <col min="21" max="21" width="14.140625" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="4"/>
+    <col min="18" max="18" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="5"/>
+    <col min="21" max="21" width="14.1640625" style="4" customWidth="1"/>
+    <col min="22" max="16384" width="11.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="31">
         <v>43745</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="E2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
@@ -913,18 +917,18 @@
       <c r="Q3" s="16"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="B4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
@@ -958,7 +962,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -976,7 +980,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1010,7 @@
       <c r="T7" s="14"/>
       <c r="U7" s="12"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1022,30 +1026,30 @@
       <c r="R8"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:21">
+      <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
@@ -1057,16 +1061,16 @@
       <c r="R9"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
+    <row r="10" spans="1:21">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -1080,7 +1084,7 @@
       <c r="R10"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:21" ht="285" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="252">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1115,7 +1119,7 @@
       <c r="R11"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="21" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1152,7 @@
       <c r="R12"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="21" t="s">
         <v>22</v>
       </c>
@@ -1181,7 +1185,7 @@
       <c r="R13"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
@@ -1214,7 +1218,7 @@
       <c r="R14"/>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
@@ -1247,7 +1251,7 @@
       <c r="R15"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
@@ -1280,7 +1284,7 @@
       <c r="R16"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="21" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1317,7 @@
       <c r="R17"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="21" t="s">
         <v>22</v>
       </c>
@@ -1346,7 +1350,7 @@
       <c r="R18"/>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="21" t="s">
         <v>22</v>
       </c>
@@ -1379,7 +1383,7 @@
       <c r="R19"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="21" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1416,7 @@
       <c r="R20"/>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="21" t="s">
         <v>22</v>
       </c>
@@ -1445,7 +1449,7 @@
       <c r="R21"/>
       <c r="S21" s="7"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="21" t="s">
         <v>22</v>
       </c>
@@ -1478,7 +1482,7 @@
       <c r="R22"/>
       <c r="S22" s="7"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="21" t="s">
         <v>22</v>
       </c>
@@ -1511,7 +1515,7 @@
       <c r="R23"/>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="21" t="s">
         <v>22</v>
       </c>
@@ -1544,7 +1548,7 @@
       <c r="R24"/>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="21" t="s">
         <v>22</v>
       </c>
@@ -1577,7 +1581,7 @@
       <c r="R25"/>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="21" t="s">
         <v>22</v>
       </c>
@@ -1610,7 +1614,7 @@
       <c r="R26"/>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="21" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1647,7 @@
       <c r="R27"/>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="21" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1680,7 @@
       <c r="R28"/>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="21" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1713,7 @@
       <c r="R29"/>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="21" t="s">
         <v>22</v>
       </c>
@@ -1742,7 +1746,7 @@
       <c r="R30"/>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="21" t="s">
         <v>22</v>
       </c>
@@ -1775,7 +1779,7 @@
       <c r="R31"/>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="21" t="s">
         <v>22</v>
       </c>
@@ -1808,7 +1812,7 @@
       <c r="R32"/>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33" s="21" t="s">
         <v>22</v>
       </c>
@@ -1841,7 +1845,7 @@
       <c r="R33"/>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34" s="21" t="s">
         <v>22</v>
       </c>
@@ -1874,7 +1878,7 @@
       <c r="R34"/>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35" s="21" t="s">
         <v>22</v>
       </c>
@@ -1907,7 +1911,7 @@
       <c r="R35"/>
       <c r="S35" s="7"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" s="21" t="s">
         <v>22</v>
       </c>
@@ -1940,7 +1944,7 @@
       <c r="R36"/>
       <c r="S36" s="7"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" s="21" t="s">
         <v>22</v>
       </c>
@@ -1973,7 +1977,7 @@
       <c r="R37"/>
       <c r="S37" s="7"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" s="21" t="s">
         <v>22</v>
       </c>
@@ -2006,7 +2010,7 @@
       <c r="R38"/>
       <c r="S38" s="7"/>
     </row>
-    <row r="39" spans="1:19" ht="300" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="252">
       <c r="A39" s="21" t="s">
         <v>22</v>
       </c>
@@ -2045,7 +2049,7 @@
       <c r="R39"/>
       <c r="S39" s="7"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="A40" s="21" t="s">
         <v>22</v>
       </c>
@@ -2072,12 +2076,12 @@
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
       <c r="N40"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
       <c r="R40"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19">
       <c r="A41" s="21" t="s">
         <v>22</v>
       </c>
@@ -2104,13 +2108,13 @@
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="28"/>
       <c r="R41"/>
       <c r="S41" s="7"/>
     </row>
-    <row r="42" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19">
       <c r="A42" s="21" t="s">
         <v>22</v>
       </c>
@@ -2137,13 +2141,13 @@
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
       <c r="R42"/>
       <c r="S42" s="7"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19">
       <c r="A43" s="21" t="s">
         <v>22</v>
       </c>
@@ -2170,13 +2174,13 @@
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="28"/>
       <c r="R43"/>
       <c r="S43" s="7"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19">
       <c r="A44" s="21" t="s">
         <v>22</v>
       </c>
@@ -2209,7 +2213,7 @@
       <c r="R44"/>
       <c r="S44" s="7"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19">
       <c r="A45" s="21" t="s">
         <v>22</v>
       </c>
@@ -2242,7 +2246,7 @@
       <c r="R45"/>
       <c r="S45" s="7"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19">
       <c r="A46" s="21" t="s">
         <v>22</v>
       </c>
@@ -2275,7 +2279,7 @@
       <c r="R46"/>
       <c r="S46" s="7"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19">
       <c r="A47" s="21" t="s">
         <v>22</v>
       </c>
@@ -2308,7 +2312,7 @@
       <c r="R47"/>
       <c r="S47" s="7"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19">
       <c r="A48" s="21" t="s">
         <v>22</v>
       </c>
@@ -2341,7 +2345,7 @@
       <c r="R48"/>
       <c r="S48" s="7"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19">
       <c r="A49" s="21" t="s">
         <v>22</v>
       </c>
@@ -2372,7 +2376,7 @@
       <c r="P49" s="15"/>
       <c r="S49" s="7"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" s="21" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2407,7 @@
       <c r="P50" s="15"/>
       <c r="S50" s="7"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="21" t="s">
         <v>22</v>
       </c>
@@ -2434,7 +2438,7 @@
       <c r="P51" s="15"/>
       <c r="S51" s="7"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="21" t="s">
         <v>22</v>
       </c>
@@ -2465,7 +2469,7 @@
       <c r="P52" s="15"/>
       <c r="S52" s="7"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19">
       <c r="A53" s="21" t="s">
         <v>22</v>
       </c>
@@ -2496,7 +2500,7 @@
       <c r="P53" s="15"/>
       <c r="S53" s="7"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" s="21" t="s">
         <v>22</v>
       </c>
@@ -2527,7 +2531,7 @@
       <c r="P54" s="15"/>
       <c r="S54" s="7"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19">
       <c r="A55" s="21" t="s">
         <v>22</v>
       </c>
@@ -2558,7 +2562,7 @@
       <c r="P55" s="15"/>
       <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19">
       <c r="A56" s="21" t="s">
         <v>22</v>
       </c>
@@ -2589,7 +2593,7 @@
       <c r="P56" s="15"/>
       <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19">
       <c r="A57" s="21" t="s">
         <v>22</v>
       </c>
@@ -2620,7 +2624,7 @@
       <c r="P57" s="15"/>
       <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19">
       <c r="A58" s="21" t="s">
         <v>22</v>
       </c>
@@ -2651,7 +2655,7 @@
       <c r="P58" s="15"/>
       <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19">
       <c r="A59" s="21" t="s">
         <v>22</v>
       </c>
@@ -2682,7 +2686,7 @@
       <c r="P59" s="15"/>
       <c r="S59" s="7"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19">
       <c r="A60" s="21" t="s">
         <v>22</v>
       </c>
@@ -2713,7 +2717,7 @@
       <c r="P60" s="15"/>
       <c r="S60" s="7"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19">
       <c r="A61" s="21" t="s">
         <v>22</v>
       </c>
@@ -2744,7 +2748,7 @@
       <c r="P61" s="15"/>
       <c r="S61" s="7"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19">
       <c r="A62" s="21" t="s">
         <v>22</v>
       </c>
@@ -2775,7 +2779,7 @@
       <c r="P62" s="15"/>
       <c r="S62" s="7"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19">
       <c r="A63" s="21" t="s">
         <v>22</v>
       </c>
@@ -2806,7 +2810,7 @@
       <c r="P63" s="15"/>
       <c r="S63" s="7"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19">
       <c r="A64" s="21" t="s">
         <v>22</v>
       </c>
@@ -2837,7 +2841,7 @@
       <c r="P64" s="15"/>
       <c r="S64" s="7"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19">
       <c r="A65" s="21" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2872,7 @@
       <c r="P65" s="15"/>
       <c r="S65" s="7"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19">
       <c r="A66" s="21" t="s">
         <v>22</v>
       </c>
@@ -2899,7 +2903,7 @@
       <c r="P66" s="15"/>
       <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19">
       <c r="A67" s="21" t="s">
         <v>22</v>
       </c>
@@ -2923,7 +2927,7 @@
       <c r="I67" s="21"/>
       <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="1:19" ht="285" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="252">
       <c r="A68" s="21" t="s">
         <v>22</v>
       </c>
@@ -2951,7 +2955,7 @@
       <c r="I68" s="21"/>
       <c r="S68" s="7"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19">
       <c r="A69" s="21" t="s">
         <v>22</v>
       </c>
@@ -2975,7 +2979,7 @@
       <c r="I69" s="21"/>
       <c r="S69" s="7"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19">
       <c r="A70" s="21" t="s">
         <v>22</v>
       </c>
@@ -2999,7 +3003,7 @@
       <c r="I70" s="21"/>
       <c r="S70" s="7"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19">
       <c r="A71" s="21" t="s">
         <v>22</v>
       </c>
@@ -3023,7 +3027,7 @@
       <c r="I71" s="21"/>
       <c r="S71" s="7"/>
     </row>
-    <row r="72" spans="1:19" ht="300" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="252">
       <c r="A72" s="21" t="s">
         <v>22</v>
       </c>
@@ -3051,7 +3055,7 @@
       <c r="I72" s="21"/>
       <c r="S72" s="7"/>
     </row>
-    <row r="73" spans="1:19" ht="300" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="252">
       <c r="A73" s="21" t="s">
         <v>22</v>
       </c>
@@ -3076,7 +3080,7 @@
       <c r="H73" s="21"/>
       <c r="I73" s="21"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19">
       <c r="A74" s="21" t="s">
         <v>22</v>
       </c>
@@ -3100,7 +3104,7 @@
       <c r="I74" s="21"/>
       <c r="S74" s="7"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19">
       <c r="A75" s="21" t="s">
         <v>22</v>
       </c>
@@ -3124,7 +3128,7 @@
       <c r="I75" s="21"/>
       <c r="S75" s="7"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19">
       <c r="A76" s="21" t="s">
         <v>22</v>
       </c>
@@ -3148,7 +3152,7 @@
       <c r="I76" s="21"/>
       <c r="S76" s="7"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19">
       <c r="A77" s="21" t="s">
         <v>22</v>
       </c>
@@ -3172,7 +3176,7 @@
       <c r="I77" s="21"/>
       <c r="S77" s="7"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19">
       <c r="A78" s="21" t="s">
         <v>22</v>
       </c>
@@ -3196,7 +3200,7 @@
       <c r="I78" s="21"/>
       <c r="S78" s="7"/>
     </row>
-    <row r="79" spans="1:19" ht="285" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="252">
       <c r="A79" s="21" t="s">
         <v>22</v>
       </c>
@@ -3222,7 +3226,7 @@
       <c r="I79" s="21"/>
       <c r="S79" s="7"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19">
       <c r="A80" s="21" t="s">
         <v>22</v>
       </c>
@@ -3246,7 +3250,7 @@
       <c r="I80" s="21"/>
       <c r="S80" s="7"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19">
       <c r="A81" s="21" t="s">
         <v>22</v>
       </c>
@@ -3270,7 +3274,7 @@
       <c r="I81" s="21"/>
       <c r="S81" s="7"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19">
       <c r="A82" s="21" t="s">
         <v>22</v>
       </c>
@@ -3294,7 +3298,7 @@
       <c r="I82" s="21"/>
       <c r="S82" s="7"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19">
       <c r="A83" s="21" t="s">
         <v>22</v>
       </c>
@@ -3318,7 +3322,7 @@
       <c r="I83" s="21"/>
       <c r="S83" s="7"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19">
       <c r="A84" s="21" t="s">
         <v>22</v>
       </c>
@@ -3342,7 +3346,7 @@
       <c r="I84" s="21"/>
       <c r="S84" s="7"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19">
       <c r="A85" s="21" t="s">
         <v>22</v>
       </c>
@@ -3366,7 +3370,7 @@
       <c r="I85" s="21"/>
       <c r="S85" s="7"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19">
       <c r="A86" s="21" t="s">
         <v>22</v>
       </c>
@@ -3390,7 +3394,7 @@
       <c r="I86" s="21"/>
       <c r="S86" s="7"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19">
       <c r="A87" s="21" t="s">
         <v>22</v>
       </c>
@@ -3414,7 +3418,7 @@
       <c r="I87" s="21"/>
       <c r="S87" s="7"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19">
       <c r="A88" s="21" t="s">
         <v>22</v>
       </c>
@@ -3438,7 +3442,7 @@
       <c r="I88" s="21"/>
       <c r="S88" s="7"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19">
       <c r="A89" s="21" t="s">
         <v>22</v>
       </c>
@@ -3462,7 +3466,7 @@
       <c r="I89" s="21"/>
       <c r="S89" s="7"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19">
       <c r="A90" s="21" t="s">
         <v>22</v>
       </c>
@@ -3486,7 +3490,7 @@
       <c r="I90" s="21"/>
       <c r="S90" s="7"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19">
       <c r="A91" s="21" t="s">
         <v>22</v>
       </c>
@@ -3510,7 +3514,7 @@
       <c r="I91" s="21"/>
       <c r="S91" s="7"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19">
       <c r="A92" s="21" t="s">
         <v>22</v>
       </c>
@@ -3534,7 +3538,7 @@
       <c r="I92" s="21"/>
       <c r="S92" s="7"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19">
       <c r="A93" s="21" t="s">
         <v>22</v>
       </c>
@@ -3558,7 +3562,7 @@
       <c r="I93" s="21"/>
       <c r="S93" s="7"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19">
       <c r="A94" s="21" t="s">
         <v>22</v>
       </c>
@@ -3582,7 +3586,7 @@
       <c r="I94" s="21"/>
       <c r="S94" s="7"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19">
       <c r="A95" s="21" t="s">
         <v>22</v>
       </c>
@@ -3605,7 +3609,7 @@
       <c r="H95" s="21"/>
       <c r="I95" s="21"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19">
       <c r="A96" s="21" t="s">
         <v>22</v>
       </c>
@@ -3629,7 +3633,7 @@
       <c r="I96" s="21"/>
       <c r="S96" s="7"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19">
       <c r="A97" s="21" t="s">
         <v>22</v>
       </c>
@@ -3653,7 +3657,7 @@
       <c r="I97" s="21"/>
       <c r="S97" s="7"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19">
       <c r="A98" s="21" t="s">
         <v>22</v>
       </c>
@@ -3677,7 +3681,7 @@
       <c r="I98" s="21"/>
       <c r="S98" s="7"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19">
       <c r="A99" s="21" t="s">
         <v>22</v>
       </c>
@@ -3701,7 +3705,7 @@
       <c r="I99" s="21"/>
       <c r="S99" s="7"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19">
       <c r="A100" s="21" t="s">
         <v>22</v>
       </c>
@@ -3725,7 +3729,7 @@
       <c r="I100" s="21"/>
       <c r="S100" s="7"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19">
       <c r="A101" s="21" t="s">
         <v>22</v>
       </c>
@@ -3749,7 +3753,7 @@
       <c r="I101" s="21"/>
       <c r="S101" s="7"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19">
       <c r="A102" s="21" t="s">
         <v>22</v>
       </c>
@@ -3773,7 +3777,7 @@
       <c r="I102" s="21"/>
       <c r="S102" s="7"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19">
       <c r="A103" s="21" t="s">
         <v>22</v>
       </c>
@@ -3797,7 +3801,7 @@
       <c r="I103" s="21"/>
       <c r="S103" s="7"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19">
       <c r="A104" s="21" t="s">
         <v>22</v>
       </c>
@@ -3821,7 +3825,7 @@
       <c r="I104" s="21"/>
       <c r="S104" s="7"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19">
       <c r="A105" s="21" t="s">
         <v>22</v>
       </c>
@@ -3845,7 +3849,7 @@
       <c r="I105" s="21"/>
       <c r="S105" s="7"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19">
       <c r="A106" s="21" t="s">
         <v>22</v>
       </c>
@@ -3869,7 +3873,7 @@
       <c r="I106" s="21"/>
       <c r="S106" s="7"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19">
       <c r="A107" s="21" t="s">
         <v>22</v>
       </c>
@@ -3893,7 +3897,7 @@
       <c r="I107" s="21"/>
       <c r="S107" s="7"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19">
       <c r="A108" s="21" t="s">
         <v>22</v>
       </c>
@@ -3917,7 +3921,7 @@
       <c r="I108" s="21"/>
       <c r="S108" s="7"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19">
       <c r="A109" s="21" t="s">
         <v>22</v>
       </c>
@@ -3941,7 +3945,7 @@
       <c r="I109" s="21"/>
       <c r="S109" s="7"/>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19">
       <c r="A110" s="21" t="s">
         <v>22</v>
       </c>
@@ -3965,7 +3969,7 @@
       <c r="I110" s="21"/>
       <c r="S110" s="7"/>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19">
       <c r="A111" s="21" t="s">
         <v>22</v>
       </c>
@@ -3989,7 +3993,7 @@
       <c r="I111" s="21"/>
       <c r="S111" s="7"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19">
       <c r="A112" s="21" t="s">
         <v>22</v>
       </c>
@@ -4012,7 +4016,7 @@
       <c r="H112" s="21"/>
       <c r="I112" s="21"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9">
       <c r="A113" s="21" t="s">
         <v>22</v>
       </c>
@@ -4035,7 +4039,7 @@
       <c r="H113" s="21"/>
       <c r="I113" s="21"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9">
       <c r="A114" s="21" t="s">
         <v>22</v>
       </c>
@@ -4058,7 +4062,7 @@
       <c r="H114" s="21"/>
       <c r="I114" s="21"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9">
       <c r="A115" s="21" t="s">
         <v>22</v>
       </c>
@@ -4081,7 +4085,7 @@
       <c r="H115" s="21"/>
       <c r="I115" s="21"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9">
       <c r="A116" s="21" t="s">
         <v>22</v>
       </c>
@@ -4104,7 +4108,7 @@
       <c r="H116" s="21"/>
       <c r="I116" s="21"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9">
       <c r="A117" s="21" t="s">
         <v>22</v>
       </c>
@@ -4127,7 +4131,7 @@
       <c r="H117" s="21"/>
       <c r="I117" s="21"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9">
       <c r="A118" s="21" t="s">
         <v>22</v>
       </c>
@@ -4150,7 +4154,7 @@
       <c r="H118" s="21"/>
       <c r="I118" s="21"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9">
       <c r="A119" s="21" t="s">
         <v>22</v>
       </c>
@@ -4173,7 +4177,7 @@
       <c r="H119" s="21"/>
       <c r="I119" s="21"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9">
       <c r="A120" s="21" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4200,7 @@
       <c r="H120" s="21"/>
       <c r="I120" s="21"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9">
       <c r="A121" s="21" t="s">
         <v>22</v>
       </c>
@@ -4219,7 +4223,7 @@
       <c r="H121" s="21"/>
       <c r="I121" s="21"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9">
       <c r="A122" s="21" t="s">
         <v>22</v>
       </c>
@@ -4242,7 +4246,7 @@
       <c r="H122" s="21"/>
       <c r="I122" s="21"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9">
       <c r="A123" s="21" t="s">
         <v>22</v>
       </c>
@@ -4265,7 +4269,7 @@
       <c r="H123" s="21"/>
       <c r="I123" s="21"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9">
       <c r="A124" s="21" t="s">
         <v>22</v>
       </c>
@@ -4288,7 +4292,7 @@
       <c r="H124" s="21"/>
       <c r="I124" s="21"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9">
       <c r="A125" s="21" t="s">
         <v>22</v>
       </c>
@@ -4311,7 +4315,7 @@
       <c r="H125" s="21"/>
       <c r="I125" s="21"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9">
       <c r="A126" s="21" t="s">
         <v>22</v>
       </c>
@@ -4334,7 +4338,7 @@
       <c r="H126" s="21"/>
       <c r="I126" s="21"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9">
       <c r="A127" s="21" t="s">
         <v>22</v>
       </c>
@@ -4357,7 +4361,7 @@
       <c r="H127" s="21"/>
       <c r="I127" s="21"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9">
       <c r="A128" s="21" t="s">
         <v>22</v>
       </c>
@@ -4380,7 +4384,7 @@
       <c r="H128" s="21"/>
       <c r="I128" s="21"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9">
       <c r="A129" s="21" t="s">
         <v>22</v>
       </c>
@@ -4403,7 +4407,7 @@
       <c r="H129" s="21"/>
       <c r="I129" s="21"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9">
       <c r="A130" s="21" t="s">
         <v>22</v>
       </c>
@@ -4426,7 +4430,7 @@
       <c r="H130" s="21"/>
       <c r="I130" s="21"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9">
       <c r="A131" s="21" t="s">
         <v>22</v>
       </c>
@@ -4449,7 +4453,7 @@
       <c r="H131" s="21"/>
       <c r="I131" s="21"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9">
       <c r="A132" s="21" t="s">
         <v>22</v>
       </c>
@@ -4472,7 +4476,7 @@
       <c r="H132" s="21"/>
       <c r="I132" s="21"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9">
       <c r="A133" s="21" t="s">
         <v>22</v>
       </c>
@@ -4495,7 +4499,7 @@
       <c r="H133" s="21"/>
       <c r="I133" s="21"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9">
       <c r="A134" s="21" t="s">
         <v>22</v>
       </c>
@@ -4518,7 +4522,7 @@
       <c r="H134" s="21"/>
       <c r="I134" s="21"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9">
       <c r="A135" s="21" t="s">
         <v>22</v>
       </c>
@@ -4541,7 +4545,7 @@
       <c r="H135" s="21"/>
       <c r="I135" s="21"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9">
       <c r="A136" s="21" t="s">
         <v>22</v>
       </c>
@@ -4564,7 +4568,7 @@
       <c r="H136" s="21"/>
       <c r="I136" s="21"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9">
       <c r="A137" s="21" t="s">
         <v>22</v>
       </c>
@@ -4587,7 +4591,7 @@
       <c r="H137" s="21"/>
       <c r="I137" s="21"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9">
       <c r="A138" s="21" t="s">
         <v>22</v>
       </c>
@@ -4610,7 +4614,7 @@
       <c r="H138" s="21"/>
       <c r="I138" s="21"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9">
       <c r="A139" s="21" t="s">
         <v>22</v>
       </c>
@@ -4633,7 +4637,7 @@
       <c r="H139" s="21"/>
       <c r="I139" s="21"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9">
       <c r="A140" s="21" t="s">
         <v>22</v>
       </c>
@@ -4656,7 +4660,7 @@
       <c r="H140" s="21"/>
       <c r="I140" s="21"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9">
       <c r="A141" s="21" t="s">
         <v>22</v>
       </c>
@@ -4679,7 +4683,7 @@
       <c r="H141" s="21"/>
       <c r="I141" s="21"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9">
       <c r="A142" s="21" t="s">
         <v>22</v>
       </c>
@@ -4702,7 +4706,7 @@
       <c r="H142" s="21"/>
       <c r="I142" s="21"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9">
       <c r="A143" s="21" t="s">
         <v>22</v>
       </c>
@@ -4725,7 +4729,7 @@
       <c r="H143" s="21"/>
       <c r="I143" s="21"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9">
       <c r="A144" s="21" t="s">
         <v>22</v>
       </c>
@@ -4748,7 +4752,7 @@
       <c r="H144" s="21"/>
       <c r="I144" s="21"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9">
       <c r="A145" s="21" t="s">
         <v>22</v>
       </c>
@@ -4771,7 +4775,7 @@
       <c r="H145" s="21"/>
       <c r="I145" s="21"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9">
       <c r="A146" s="21" t="s">
         <v>22</v>
       </c>
@@ -4794,7 +4798,7 @@
       <c r="H146" s="21"/>
       <c r="I146" s="21"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9">
       <c r="A147" s="21" t="s">
         <v>22</v>
       </c>
@@ -4817,7 +4821,7 @@
       <c r="H147" s="21"/>
       <c r="I147" s="21"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9">
       <c r="A148" s="21" t="s">
         <v>22</v>
       </c>
@@ -4840,7 +4844,7 @@
       <c r="H148" s="21"/>
       <c r="I148" s="21"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9">
       <c r="A149" s="21" t="s">
         <v>22</v>
       </c>
@@ -4863,7 +4867,7 @@
       <c r="H149" s="21"/>
       <c r="I149" s="21"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9">
       <c r="A150" s="21" t="s">
         <v>22</v>
       </c>
@@ -4886,7 +4890,7 @@
       <c r="H150" s="21"/>
       <c r="I150" s="21"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9">
       <c r="A151" s="21" t="s">
         <v>22</v>
       </c>
@@ -4909,7 +4913,7 @@
       <c r="H151" s="21"/>
       <c r="I151" s="21"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9">
       <c r="A152" s="21" t="s">
         <v>22</v>
       </c>
@@ -4932,7 +4936,7 @@
       <c r="H152" s="21"/>
       <c r="I152" s="21"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9">
       <c r="A153" s="21" t="s">
         <v>22</v>
       </c>
@@ -4955,7 +4959,7 @@
       <c r="H153" s="21"/>
       <c r="I153" s="21"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9">
       <c r="A154" s="21" t="s">
         <v>22</v>
       </c>
@@ -4978,7 +4982,7 @@
       <c r="H154" s="21"/>
       <c r="I154" s="21"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9">
       <c r="A155" s="21" t="s">
         <v>22</v>
       </c>
@@ -5001,7 +5005,7 @@
       <c r="H155" s="21"/>
       <c r="I155" s="21"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9">
       <c r="A156" s="21" t="s">
         <v>22</v>
       </c>
@@ -5024,7 +5028,7 @@
       <c r="H156" s="21"/>
       <c r="I156" s="21"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9">
       <c r="A157" s="21" t="s">
         <v>22</v>
       </c>
@@ -5047,7 +5051,7 @@
       <c r="H157" s="21"/>
       <c r="I157" s="21"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9">
       <c r="A158" s="21" t="s">
         <v>22</v>
       </c>
@@ -5070,7 +5074,7 @@
       <c r="H158" s="21"/>
       <c r="I158" s="21"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9">
       <c r="A159" s="21" t="s">
         <v>22</v>
       </c>
@@ -5093,7 +5097,7 @@
       <c r="H159" s="21"/>
       <c r="I159" s="21"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9">
       <c r="A160" s="21" t="s">
         <v>22</v>
       </c>
@@ -5116,7 +5120,7 @@
       <c r="H160" s="21"/>
       <c r="I160" s="21"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9">
       <c r="A161" s="21" t="s">
         <v>22</v>
       </c>
@@ -5139,7 +5143,7 @@
       <c r="H161" s="21"/>
       <c r="I161" s="21"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9">
       <c r="A162" s="21" t="s">
         <v>22</v>
       </c>
@@ -5162,7 +5166,7 @@
       <c r="H162" s="21"/>
       <c r="I162" s="21"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9">
       <c r="A163" s="21" t="s">
         <v>22</v>
       </c>
@@ -5185,7 +5189,7 @@
       <c r="H163" s="21"/>
       <c r="I163" s="21"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9">
       <c r="A164" s="21" t="s">
         <v>22</v>
       </c>
@@ -5208,7 +5212,7 @@
       <c r="H164" s="21"/>
       <c r="I164" s="21"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9">
       <c r="A165" s="21" t="s">
         <v>22</v>
       </c>
@@ -5231,7 +5235,7 @@
       <c r="H165" s="21"/>
       <c r="I165" s="21"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9">
       <c r="A166" s="21" t="s">
         <v>22</v>
       </c>
@@ -5254,7 +5258,7 @@
       <c r="H166" s="21"/>
       <c r="I166" s="21"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9">
       <c r="A167" s="21" t="s">
         <v>22</v>
       </c>
@@ -5277,7 +5281,7 @@
       <c r="H167" s="21"/>
       <c r="I167" s="21"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9">
       <c r="A168" s="21" t="s">
         <v>22</v>
       </c>
@@ -5300,7 +5304,7 @@
       <c r="H168" s="21"/>
       <c r="I168" s="21"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9">
       <c r="A169" s="21" t="s">
         <v>22</v>
       </c>
@@ -5323,7 +5327,7 @@
       <c r="H169" s="21"/>
       <c r="I169" s="21"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9">
       <c r="A170" s="21" t="s">
         <v>22</v>
       </c>
@@ -5346,7 +5350,7 @@
       <c r="H170" s="21"/>
       <c r="I170" s="21"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9">
       <c r="A171" s="21" t="s">
         <v>22</v>
       </c>
@@ -5369,7 +5373,7 @@
       <c r="H171" s="21"/>
       <c r="I171" s="21"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9">
       <c r="A172" s="21" t="s">
         <v>22</v>
       </c>
@@ -5392,7 +5396,7 @@
       <c r="H172" s="21"/>
       <c r="I172" s="21"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9">
       <c r="A173" s="21" t="s">
         <v>22</v>
       </c>
@@ -5415,7 +5419,7 @@
       <c r="H173" s="21"/>
       <c r="I173" s="21"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9">
       <c r="A174" s="21" t="s">
         <v>22</v>
       </c>
@@ -5438,7 +5442,7 @@
       <c r="H174" s="21"/>
       <c r="I174" s="21"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9">
       <c r="A175" s="21" t="s">
         <v>22</v>
       </c>
@@ -5461,7 +5465,7 @@
       <c r="H175" s="21"/>
       <c r="I175" s="21"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9">
       <c r="A176" s="21" t="s">
         <v>22</v>
       </c>
@@ -5484,7 +5488,7 @@
       <c r="H176" s="21"/>
       <c r="I176" s="21"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9">
       <c r="A177" s="21" t="s">
         <v>22</v>
       </c>
@@ -5507,7 +5511,7 @@
       <c r="H177" s="21"/>
       <c r="I177" s="21"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9">
       <c r="A178" s="21" t="s">
         <v>22</v>
       </c>
@@ -5530,7 +5534,7 @@
       <c r="H178" s="21"/>
       <c r="I178" s="21"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9">
       <c r="A179" s="21" t="s">
         <v>22</v>
       </c>
@@ -5553,7 +5557,7 @@
       <c r="H179" s="21"/>
       <c r="I179" s="21"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9">
       <c r="A180" s="21" t="s">
         <v>22</v>
       </c>
@@ -5576,7 +5580,7 @@
       <c r="H180" s="21"/>
       <c r="I180" s="21"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9">
       <c r="A181" s="21" t="s">
         <v>22</v>
       </c>
@@ -5599,7 +5603,7 @@
       <c r="H181" s="21"/>
       <c r="I181" s="21"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9">
       <c r="A182" s="21" t="s">
         <v>22</v>
       </c>
@@ -5622,7 +5626,7 @@
       <c r="H182" s="21"/>
       <c r="I182" s="21"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9">
       <c r="A183" s="21" t="s">
         <v>22</v>
       </c>
@@ -5645,7 +5649,7 @@
       <c r="H183" s="21"/>
       <c r="I183" s="21"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9">
       <c r="A184" s="21" t="s">
         <v>22</v>
       </c>
@@ -5668,7 +5672,7 @@
       <c r="H184" s="21"/>
       <c r="I184" s="21"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9">
       <c r="A185" s="21" t="s">
         <v>22</v>
       </c>
@@ -5691,7 +5695,7 @@
       <c r="H185" s="21"/>
       <c r="I185" s="21"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9">
       <c r="A186" s="21" t="s">
         <v>22</v>
       </c>
@@ -5714,7 +5718,7 @@
       <c r="H186" s="21"/>
       <c r="I186" s="21"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9">
       <c r="A187" s="21" t="s">
         <v>22</v>
       </c>
@@ -5737,7 +5741,7 @@
       <c r="H187" s="21"/>
       <c r="I187" s="21"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9">
       <c r="A188" s="21" t="s">
         <v>22</v>
       </c>
@@ -5760,7 +5764,7 @@
       <c r="H188" s="21"/>
       <c r="I188" s="21"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9">
       <c r="A189" s="21" t="s">
         <v>22</v>
       </c>
@@ -5783,7 +5787,7 @@
       <c r="H189" s="21"/>
       <c r="I189" s="21"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9">
       <c r="A190" s="21" t="s">
         <v>22</v>
       </c>
@@ -5806,7 +5810,7 @@
       <c r="H190" s="21"/>
       <c r="I190" s="21"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9">
       <c r="A191" s="21" t="s">
         <v>22</v>
       </c>
@@ -5829,7 +5833,7 @@
       <c r="H191" s="21"/>
       <c r="I191" s="21"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9">
       <c r="A192" s="21" t="s">
         <v>22</v>
       </c>
@@ -5852,7 +5856,7 @@
       <c r="H192" s="21"/>
       <c r="I192" s="21"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9">
       <c r="A193" s="21" t="s">
         <v>22</v>
       </c>
@@ -5875,7 +5879,7 @@
       <c r="H193" s="21"/>
       <c r="I193" s="21"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9">
       <c r="A194" s="21" t="s">
         <v>22</v>
       </c>
@@ -5898,7 +5902,7 @@
       <c r="H194" s="21"/>
       <c r="I194" s="21"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9">
       <c r="A195" s="21" t="s">
         <v>22</v>
       </c>
@@ -5921,7 +5925,7 @@
       <c r="H195" s="21"/>
       <c r="I195" s="21"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9">
       <c r="A196" s="21" t="s">
         <v>22</v>
       </c>
@@ -5944,7 +5948,7 @@
       <c r="H196" s="21"/>
       <c r="I196" s="21"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9">
       <c r="A197" s="21" t="s">
         <v>22</v>
       </c>
@@ -5967,7 +5971,7 @@
       <c r="H197" s="21"/>
       <c r="I197" s="21"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9">
       <c r="A198" s="21" t="s">
         <v>22</v>
       </c>
@@ -5990,7 +5994,7 @@
       <c r="H198" s="21"/>
       <c r="I198" s="21"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9">
       <c r="A199" s="21" t="s">
         <v>22</v>
       </c>
@@ -6013,7 +6017,7 @@
       <c r="H199" s="21"/>
       <c r="I199" s="21"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9">
       <c r="A200" s="21" t="s">
         <v>22</v>
       </c>
@@ -6036,7 +6040,7 @@
       <c r="H200" s="21"/>
       <c r="I200" s="21"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9">
       <c r="A201" s="21" t="s">
         <v>22</v>
       </c>
@@ -6059,7 +6063,7 @@
       <c r="H201" s="21"/>
       <c r="I201" s="21"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9">
       <c r="A202" s="21" t="s">
         <v>22</v>
       </c>
@@ -6082,7 +6086,7 @@
       <c r="H202" s="21"/>
       <c r="I202" s="21"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9">
       <c r="A203" s="21" t="s">
         <v>22</v>
       </c>
@@ -6105,7 +6109,7 @@
       <c r="H203" s="21"/>
       <c r="I203" s="21"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9">
       <c r="A204" s="21" t="s">
         <v>22</v>
       </c>
@@ -6128,7 +6132,7 @@
       <c r="H204" s="21"/>
       <c r="I204" s="21"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9">
       <c r="A205" s="21" t="s">
         <v>22</v>
       </c>
@@ -6151,7 +6155,7 @@
       <c r="H205" s="21"/>
       <c r="I205" s="21"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9">
       <c r="A206" s="21" t="s">
         <v>22</v>
       </c>
@@ -6174,7 +6178,7 @@
       <c r="H206" s="21"/>
       <c r="I206" s="21"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9">
       <c r="A207" s="21" t="s">
         <v>22</v>
       </c>
@@ -6197,7 +6201,7 @@
       <c r="H207" s="21"/>
       <c r="I207" s="21"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9">
       <c r="A208" s="21" t="s">
         <v>22</v>
       </c>
@@ -6220,7 +6224,7 @@
       <c r="H208" s="21"/>
       <c r="I208" s="21"/>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9">
       <c r="A209" s="21" t="s">
         <v>22</v>
       </c>
@@ -6243,7 +6247,7 @@
       <c r="H209" s="21"/>
       <c r="I209" s="21"/>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9">
       <c r="A210" s="21" t="s">
         <v>22</v>
       </c>
@@ -6266,7 +6270,7 @@
       <c r="H210" s="21"/>
       <c r="I210" s="21"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9">
       <c r="A211" s="21" t="s">
         <v>22</v>
       </c>
@@ -6289,7 +6293,7 @@
       <c r="H211" s="21"/>
       <c r="I211" s="21"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9">
       <c r="A212" s="21" t="s">
         <v>22</v>
       </c>
@@ -6312,7 +6316,7 @@
       <c r="H212" s="21"/>
       <c r="I212" s="21"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9">
       <c r="A213" s="21" t="s">
         <v>22</v>
       </c>
@@ -6335,7 +6339,7 @@
       <c r="H213" s="21"/>
       <c r="I213" s="21"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9">
       <c r="A214" s="21" t="s">
         <v>22</v>
       </c>
@@ -6358,7 +6362,7 @@
       <c r="H214" s="21"/>
       <c r="I214" s="21"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9">
       <c r="A215" s="21" t="s">
         <v>22</v>
       </c>
@@ -6381,7 +6385,7 @@
       <c r="H215" s="21"/>
       <c r="I215" s="21"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9">
       <c r="A216" s="21" t="s">
         <v>22</v>
       </c>
@@ -6404,7 +6408,7 @@
       <c r="H216" s="21"/>
       <c r="I216" s="21"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9">
       <c r="A217" s="21" t="s">
         <v>22</v>
       </c>
@@ -6427,7 +6431,7 @@
       <c r="H217" s="21"/>
       <c r="I217" s="21"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9">
       <c r="A218" s="21" t="s">
         <v>22</v>
       </c>
@@ -6450,7 +6454,7 @@
       <c r="H218" s="21"/>
       <c r="I218" s="21"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9">
       <c r="A219" s="21" t="s">
         <v>22</v>
       </c>
@@ -6473,7 +6477,7 @@
       <c r="H219" s="21"/>
       <c r="I219" s="21"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9">
       <c r="A220" s="21" t="s">
         <v>22</v>
       </c>
@@ -6496,7 +6500,7 @@
       <c r="H220" s="21"/>
       <c r="I220" s="21"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9">
       <c r="A221" s="21" t="s">
         <v>22</v>
       </c>
@@ -6519,7 +6523,7 @@
       <c r="H221" s="21"/>
       <c r="I221" s="21"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9">
       <c r="A222" s="21" t="s">
         <v>22</v>
       </c>
@@ -6542,7 +6546,7 @@
       <c r="H222" s="21"/>
       <c r="I222" s="21"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9">
       <c r="A223" s="21" t="s">
         <v>22</v>
       </c>
@@ -6565,7 +6569,7 @@
       <c r="H223" s="21"/>
       <c r="I223" s="21"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9">
       <c r="A224" s="21" t="s">
         <v>22</v>
       </c>
@@ -6588,7 +6592,7 @@
       <c r="H224" s="21"/>
       <c r="I224" s="21"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9">
       <c r="A225" s="21" t="s">
         <v>22</v>
       </c>
@@ -6611,7 +6615,7 @@
       <c r="H225" s="21"/>
       <c r="I225" s="21"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9">
       <c r="A226" s="21" t="s">
         <v>22</v>
       </c>
@@ -6634,7 +6638,7 @@
       <c r="H226" s="21"/>
       <c r="I226" s="21"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9">
       <c r="A227" s="21" t="s">
         <v>22</v>
       </c>
@@ -6657,7 +6661,7 @@
       <c r="H227" s="21"/>
       <c r="I227" s="21"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9">
       <c r="A228" s="21" t="s">
         <v>22</v>
       </c>
@@ -6680,7 +6684,7 @@
       <c r="H228" s="21"/>
       <c r="I228" s="21"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9">
       <c r="A229" s="21" t="s">
         <v>22</v>
       </c>
@@ -6703,7 +6707,7 @@
       <c r="H229" s="21"/>
       <c r="I229" s="21"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9">
       <c r="A230" s="21" t="s">
         <v>22</v>
       </c>
@@ -6726,7 +6730,7 @@
       <c r="H230" s="21"/>
       <c r="I230" s="21"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9">
       <c r="A231" s="21" t="s">
         <v>22</v>
       </c>
@@ -6749,7 +6753,7 @@
       <c r="H231" s="21"/>
       <c r="I231" s="21"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9">
       <c r="A232" s="21" t="s">
         <v>22</v>
       </c>
@@ -6772,7 +6776,7 @@
       <c r="H232" s="21"/>
       <c r="I232" s="21"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9">
       <c r="A233" s="21" t="s">
         <v>22</v>
       </c>
@@ -6795,7 +6799,7 @@
       <c r="H233" s="21"/>
       <c r="I233" s="21"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9">
       <c r="A234" s="21" t="s">
         <v>22</v>
       </c>
@@ -6818,7 +6822,7 @@
       <c r="H234" s="21"/>
       <c r="I234" s="21"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9">
       <c r="A235" s="21" t="s">
         <v>22</v>
       </c>
@@ -6841,7 +6845,7 @@
       <c r="H235" s="21"/>
       <c r="I235" s="21"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9">
       <c r="A236" s="21" t="s">
         <v>22</v>
       </c>
@@ -6864,7 +6868,7 @@
       <c r="H236" s="21"/>
       <c r="I236" s="21"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9">
       <c r="A237" s="21" t="s">
         <v>22</v>
       </c>
@@ -6887,7 +6891,7 @@
       <c r="H237" s="21"/>
       <c r="I237" s="21"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9">
       <c r="A238" s="21" t="s">
         <v>22</v>
       </c>
@@ -6910,7 +6914,7 @@
       <c r="H238" s="21"/>
       <c r="I238" s="21"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9">
       <c r="A239" s="21" t="s">
         <v>22</v>
       </c>
@@ -6933,7 +6937,7 @@
       <c r="H239" s="21"/>
       <c r="I239" s="21"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9">
       <c r="A240" s="21" t="s">
         <v>22</v>
       </c>
@@ -6956,7 +6960,7 @@
       <c r="H240" s="21"/>
       <c r="I240" s="21"/>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9">
       <c r="A241" s="21" t="s">
         <v>22</v>
       </c>
@@ -6979,7 +6983,7 @@
       <c r="H241" s="21"/>
       <c r="I241" s="21"/>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9">
       <c r="A242" s="21" t="s">
         <v>22</v>
       </c>
@@ -7002,7 +7006,7 @@
       <c r="H242" s="21"/>
       <c r="I242" s="21"/>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9">
       <c r="A243" s="21" t="s">
         <v>22</v>
       </c>
@@ -7025,7 +7029,7 @@
       <c r="H243" s="21"/>
       <c r="I243" s="21"/>
     </row>
-    <row r="244" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="252">
       <c r="A244" s="21" t="s">
         <v>22</v>
       </c>
@@ -7050,7 +7054,7 @@
       <c r="H244" s="21"/>
       <c r="I244" s="21"/>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9">
       <c r="A245" s="21" t="s">
         <v>22</v>
       </c>
@@ -7073,7 +7077,7 @@
       <c r="H245" s="21"/>
       <c r="I245" s="21"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9">
       <c r="A246" s="21" t="s">
         <v>22</v>
       </c>
@@ -7096,7 +7100,7 @@
       <c r="H246" s="21"/>
       <c r="I246" s="21"/>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9">
       <c r="A247" s="21" t="s">
         <v>22</v>
       </c>
@@ -7119,7 +7123,7 @@
       <c r="H247" s="21"/>
       <c r="I247" s="21"/>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9">
       <c r="A248" s="21" t="s">
         <v>22</v>
       </c>
@@ -7142,7 +7146,7 @@
       <c r="H248" s="21"/>
       <c r="I248" s="21"/>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9">
       <c r="A249" s="21" t="s">
         <v>22</v>
       </c>
@@ -7165,7 +7169,7 @@
       <c r="H249" s="21"/>
       <c r="I249" s="21"/>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9">
       <c r="A250" s="21" t="s">
         <v>22</v>
       </c>
@@ -7188,7 +7192,7 @@
       <c r="H250" s="21"/>
       <c r="I250" s="21"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9">
       <c r="A251" s="21" t="s">
         <v>22</v>
       </c>
@@ -7211,7 +7215,7 @@
       <c r="H251" s="21"/>
       <c r="I251" s="21"/>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9">
       <c r="A252" s="21" t="s">
         <v>22</v>
       </c>
@@ -7234,7 +7238,7 @@
       <c r="H252" s="21"/>
       <c r="I252" s="21"/>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9">
       <c r="A253" s="21" t="s">
         <v>22</v>
       </c>
@@ -7257,7 +7261,7 @@
       <c r="H253" s="21"/>
       <c r="I253" s="21"/>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9">
       <c r="A254" s="21" t="s">
         <v>22</v>
       </c>
@@ -7280,7 +7284,7 @@
       <c r="H254" s="21"/>
       <c r="I254" s="21"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9">
       <c r="A255" s="21" t="s">
         <v>22</v>
       </c>
@@ -7303,7 +7307,7 @@
       <c r="H255" s="21"/>
       <c r="I255" s="21"/>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9">
       <c r="A256" s="21" t="s">
         <v>22</v>
       </c>
@@ -7326,7 +7330,7 @@
       <c r="H256" s="21"/>
       <c r="I256" s="21"/>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9">
       <c r="A257" s="21" t="s">
         <v>22</v>
       </c>
@@ -7349,7 +7353,7 @@
       <c r="H257" s="21"/>
       <c r="I257" s="21"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9">
       <c r="A258" s="21" t="s">
         <v>22</v>
       </c>
@@ -7372,7 +7376,7 @@
       <c r="H258" s="21"/>
       <c r="I258" s="21"/>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9">
       <c r="A259" s="21" t="s">
         <v>22</v>
       </c>
@@ -7395,7 +7399,7 @@
       <c r="H259" s="21"/>
       <c r="I259" s="21"/>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9">
       <c r="A260" s="21" t="s">
         <v>22</v>
       </c>
@@ -7418,7 +7422,7 @@
       <c r="H260" s="21"/>
       <c r="I260" s="21"/>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9">
       <c r="A261" s="21" t="s">
         <v>22</v>
       </c>
@@ -7441,7 +7445,7 @@
       <c r="H261" s="21"/>
       <c r="I261" s="21"/>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9">
       <c r="A262" s="21" t="s">
         <v>22</v>
       </c>
@@ -7464,7 +7468,7 @@
       <c r="H262" s="21"/>
       <c r="I262" s="21"/>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9">
       <c r="A263" s="21" t="s">
         <v>22</v>
       </c>
@@ -7487,7 +7491,7 @@
       <c r="H263" s="21"/>
       <c r="I263" s="21"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9">
       <c r="A264" s="21" t="s">
         <v>22</v>
       </c>
@@ -7510,7 +7514,7 @@
       <c r="H264" s="21"/>
       <c r="I264" s="21"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9">
       <c r="A265" s="21" t="s">
         <v>22</v>
       </c>
@@ -7533,7 +7537,7 @@
       <c r="H265" s="21"/>
       <c r="I265" s="21"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9">
       <c r="A266" s="21" t="s">
         <v>22</v>
       </c>
@@ -7556,7 +7560,7 @@
       <c r="H266" s="21"/>
       <c r="I266" s="21"/>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9">
       <c r="A267" s="21" t="s">
         <v>22</v>
       </c>
@@ -7579,7 +7583,7 @@
       <c r="H267" s="21"/>
       <c r="I267" s="21"/>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9">
       <c r="A268" s="21" t="s">
         <v>22</v>
       </c>
@@ -7602,7 +7606,7 @@
       <c r="H268" s="21"/>
       <c r="I268" s="21"/>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9">
       <c r="A269" s="21" t="s">
         <v>22</v>
       </c>
@@ -7625,7 +7629,7 @@
       <c r="H269" s="21"/>
       <c r="I269" s="21"/>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9">
       <c r="A270" s="21" t="s">
         <v>22</v>
       </c>
@@ -7648,7 +7652,7 @@
       <c r="H270" s="21"/>
       <c r="I270" s="21"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9">
       <c r="A271" s="21" t="s">
         <v>22</v>
       </c>
@@ -7671,7 +7675,7 @@
       <c r="H271" s="21"/>
       <c r="I271" s="21"/>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9">
       <c r="A272" s="21" t="s">
         <v>22</v>
       </c>
@@ -7694,7 +7698,7 @@
       <c r="H272" s="21"/>
       <c r="I272" s="21"/>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9">
       <c r="A273" s="21" t="s">
         <v>22</v>
       </c>
@@ -7717,7 +7721,7 @@
       <c r="H273" s="21"/>
       <c r="I273" s="21"/>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9">
       <c r="A274" s="21" t="s">
         <v>22</v>
       </c>
@@ -7740,7 +7744,7 @@
       <c r="H274" s="21"/>
       <c r="I274" s="21"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9">
       <c r="A275" s="21" t="s">
         <v>22</v>
       </c>
@@ -7763,7 +7767,7 @@
       <c r="H275" s="21"/>
       <c r="I275" s="21"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9">
       <c r="A276" s="21" t="s">
         <v>22</v>
       </c>
@@ -7786,7 +7790,7 @@
       <c r="H276" s="21"/>
       <c r="I276" s="21"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9">
       <c r="A277" s="21" t="s">
         <v>22</v>
       </c>
@@ -7809,7 +7813,7 @@
       <c r="H277" s="21"/>
       <c r="I277" s="21"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9">
       <c r="A278" s="21" t="s">
         <v>22</v>
       </c>
@@ -7832,7 +7836,7 @@
       <c r="H278" s="21"/>
       <c r="I278" s="21"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9">
       <c r="A279" s="21" t="s">
         <v>22</v>
       </c>
@@ -7855,7 +7859,7 @@
       <c r="H279" s="21"/>
       <c r="I279" s="21"/>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9">
       <c r="A280" s="21" t="s">
         <v>22</v>
       </c>
@@ -7878,7 +7882,7 @@
       <c r="H280" s="21"/>
       <c r="I280" s="21"/>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9">
       <c r="A281" s="21" t="s">
         <v>22</v>
       </c>
@@ -7901,7 +7905,7 @@
       <c r="H281" s="21"/>
       <c r="I281" s="21"/>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9">
       <c r="A282" s="21" t="s">
         <v>22</v>
       </c>
@@ -7924,7 +7928,7 @@
       <c r="H282" s="21"/>
       <c r="I282" s="21"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9">
       <c r="A283" s="21" t="s">
         <v>22</v>
       </c>
@@ -7947,7 +7951,7 @@
       <c r="H283" s="21"/>
       <c r="I283" s="21"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9">
       <c r="A284" s="21" t="s">
         <v>22</v>
       </c>
@@ -7970,7 +7974,7 @@
       <c r="H284" s="21"/>
       <c r="I284" s="21"/>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9">
       <c r="A285" s="21" t="s">
         <v>22</v>
       </c>
@@ -7993,7 +7997,7 @@
       <c r="H285" s="21"/>
       <c r="I285" s="21"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9">
       <c r="A286" s="21" t="s">
         <v>22</v>
       </c>
@@ -8016,7 +8020,7 @@
       <c r="H286" s="21"/>
       <c r="I286" s="21"/>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9">
       <c r="A287" s="21" t="s">
         <v>22</v>
       </c>
@@ -8039,7 +8043,7 @@
       <c r="H287" s="21"/>
       <c r="I287" s="21"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9">
       <c r="A288" s="21" t="s">
         <v>22</v>
       </c>
@@ -8064,11 +8068,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:I10"/>
     <mergeCell ref="O42:Q42"/>
     <mergeCell ref="O43:Q43"/>
     <mergeCell ref="E2:I2"/>
@@ -8081,37 +8080,56 @@
     <mergeCell ref="O41:Q41"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:I10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G68" r:id="rId2" xr:uid="{3AC94A96-80C9-422E-8D6E-0B420F576A8C}"/>
-    <hyperlink ref="H72" r:id="rId3" xr:uid="{AA17A346-A3CF-4885-AABC-ECF4CFC0235F}"/>
+    <hyperlink ref="G39" r:id="rId1"/>
+    <hyperlink ref="G68" r:id="rId2"/>
+    <hyperlink ref="H72" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId4"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>